<commit_message>
add, edit, del functionality covered
</commit_message>
<xml_diff>
--- a/Testdata/LiveRef/ManageSourceData/AUT_2022_Template - old.xlsx
+++ b/Testdata/LiveRef/ManageSourceData/AUT_2022_Template - old.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swetham\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\LiveRef\ManageSourceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BBC6D7-32AF-4178-AEA4-BBC3EDA1438F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF2B73D-77AF-4752-B6BF-6802ED14AB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -119,10 +119,10 @@
     <t>Main_Results</t>
   </si>
   <si>
-    <t>Category of Evidence</t>
-  </si>
-  <si>
     <t>testdemo</t>
+  </si>
+  <si>
+    <t>Study Type/GVD Chapter</t>
   </si>
 </sst>
 </file>
@@ -576,32 +576,32 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
-    <col min="9" max="9" width="18.1796875" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" customWidth="1"/>
-    <col min="14" max="14" width="18.26953125" customWidth="1"/>
-    <col min="15" max="15" width="14.453125" customWidth="1"/>
-    <col min="16" max="16" width="12.1796875" customWidth="1"/>
-    <col min="17" max="17" width="13.1796875" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" customWidth="1"/>
+    <col min="14" max="14" width="18.21875" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" customWidth="1"/>
+    <col min="17" max="17" width="13.21875" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -627,7 +627,7 @@
         <v>20</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>21</v>
@@ -657,7 +657,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -665,28 +665,28 @@
         <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>14</v>
@@ -698,188 +698,188 @@
         <v>1234</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="18" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="19" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="68" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="77" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="82" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="83" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="85" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="86" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="87" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="88" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="89" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="90" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="91" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="92" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="93" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="94" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="95" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="96" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="97" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="99" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="100" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="101" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="102" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="103" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="104" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="105" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="106" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="107" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="108" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="109" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="110" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="111" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="112" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="113" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="114" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="115" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="116" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="117" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="118" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="119" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="120" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="121" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="122" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="123" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="124" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="125" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="126" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="127" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="128" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="129" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="130" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="131" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="132" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="133" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="134" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="135" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="136" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="137" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="138" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="139" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="140" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="141" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="142" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="143" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="144" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="145" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="146" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="147" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="148" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="149" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="150" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="151" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="152" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="153" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="154" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="155" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="156" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="157" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="158" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="159" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="160" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="161" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="162" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="163" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="164" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="165" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="166" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="167" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="168" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="169" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="130" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="132" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="135" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="136" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="137" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="141" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="164" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -892,7 +892,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -904,7 +904,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -918,9 +918,9 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1" t="s">
         <v>17</v>
       </c>
@@ -931,21 +931,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BBCC0D8A7D6FE0469D1BA865BCA834CE" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="918213ac96e7cfc7550203515069d461">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c267871d-e92d-4bec-a268-edb541a91654" xmlns:ns3="4654e9f1-a236-4d55-b6c2-932c37e5d109" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="689c50ae291abccbfd9694277c471f87" ns2:_="" ns3:_="">
     <xsd:import namespace="c267871d-e92d-4bec-a268-edb541a91654"/>
@@ -1162,10 +1147,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7BAB9B7-7148-4FC2-919A-8F6E750DF90B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBB960FF-F5B0-418D-807A-120B8EC44EF5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c267871d-e92d-4bec-a268-edb541a91654"/>
+    <ds:schemaRef ds:uri="4654e9f1-a236-4d55-b6c2-932c37e5d109"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1188,20 +1199,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBB960FF-F5B0-418D-807A-120B8EC44EF5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7BAB9B7-7148-4FC2-919A-8F6E750DF90B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c267871d-e92d-4bec-a268-edb541a91654"/>
-    <ds:schemaRef ds:uri="4654e9f1-a236-4d55-b6c2-932c37e5d109"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>